<commit_message>
Correct values for biogenic methane.
</commit_message>
<xml_diff>
--- a/premise_gwp/data/lcia_gwp2021_100a.xlsx
+++ b/premise_gwp/data/lcia_gwp2021_100a.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise_gwp/premise_gwp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38647006-5A68-844C-B09E-118510B5A1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C37BE2-A809-FF47-A14E-7B30E4F7DDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$253</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$249</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="65">
   <si>
     <t>name</t>
   </si>
@@ -594,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C253"/>
+  <dimension ref="A1:C249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="C196" sqref="C196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2715,7 +2715,8 @@
         <v>49</v>
       </c>
       <c r="C192">
-        <v>27</v>
+        <f>C177-2.75</f>
+        <v>27.05</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
@@ -2726,7 +2727,8 @@
         <v>47</v>
       </c>
       <c r="C193">
-        <v>29.8</v>
+        <f>C178-2.75</f>
+        <v>27.05</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
@@ -2737,7 +2739,8 @@
         <v>50</v>
       </c>
       <c r="C194">
-        <v>29.8</v>
+        <f>C179-2.75</f>
+        <v>27.05</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
@@ -2748,7 +2751,8 @@
         <v>46</v>
       </c>
       <c r="C195">
-        <v>29.8</v>
+        <f>C180-2.75</f>
+        <v>27.05</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
@@ -2759,51 +2763,52 @@
         <v>48</v>
       </c>
       <c r="C196">
-        <v>29.8</v>
+        <f>C181-2.75</f>
+        <v>27.05</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B197" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C197">
-        <v>27</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B198" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C198">
-        <v>27</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B199" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C199">
-        <v>27</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B200" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C200">
-        <v>27</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
@@ -2811,7 +2816,7 @@
         <v>38</v>
       </c>
       <c r="B201" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C201">
         <v>2200</v>
@@ -2819,46 +2824,46 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B202" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C202">
-        <v>2200</v>
+        <v>7380</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B203" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C203">
-        <v>2200</v>
+        <v>7380</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B204" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C204">
-        <v>2200</v>
+        <v>7380</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B205" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C205">
-        <v>2200</v>
+        <v>7380</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
@@ -2866,7 +2871,7 @@
         <v>39</v>
       </c>
       <c r="B206" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C206">
         <v>7380</v>
@@ -2874,46 +2879,46 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B207" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C207">
-        <v>7380</v>
+        <v>6230</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B208" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C208">
-        <v>7380</v>
+        <v>6230</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B209" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C209">
-        <v>7380</v>
+        <v>6230</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B210" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C210">
-        <v>7380</v>
+        <v>6230</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
@@ -2921,7 +2926,7 @@
         <v>40</v>
       </c>
       <c r="B211" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C211">
         <v>6230</v>
@@ -2929,46 +2934,46 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B212" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C212">
-        <v>6230</v>
+        <v>14600</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B213" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C213">
-        <v>6230</v>
+        <v>14600</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B214" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C214">
-        <v>6230</v>
+        <v>14600</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B215" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C215">
-        <v>6230</v>
+        <v>14600</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
@@ -2976,7 +2981,7 @@
         <v>41</v>
       </c>
       <c r="B216" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C216">
         <v>14600</v>
@@ -2984,46 +2989,46 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B217" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C217">
-        <v>14600</v>
+        <v>0.48099999999999998</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B218" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C218">
-        <v>14600</v>
+        <v>0.48099999999999998</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B219" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C219">
-        <v>14600</v>
+        <v>0.48099999999999998</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B220" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C220">
-        <v>14600</v>
+        <v>0.48099999999999998</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
@@ -3031,7 +3036,7 @@
         <v>61</v>
       </c>
       <c r="B221" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C221">
         <v>0.48099999999999998</v>
@@ -3039,57 +3044,57 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B222" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C222">
-        <v>0.48099999999999998</v>
+        <v>-10.8</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B223" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C223">
-        <v>0.48099999999999998</v>
+        <v>17400</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B224" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C224">
-        <v>0.48099999999999998</v>
+        <v>17400</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B225" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C225">
-        <v>0.48099999999999998</v>
+        <v>17400</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B226" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C226">
-        <v>-10.8</v>
+        <v>17400</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
@@ -3097,7 +3102,7 @@
         <v>43</v>
       </c>
       <c r="B227" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C227">
         <v>17400</v>
@@ -3105,57 +3110,57 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B228" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C228">
-        <v>17400</v>
+        <v>9220</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B229" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C229">
-        <v>17400</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B230" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C230">
-        <v>17400</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B231" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C231">
-        <v>17400</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B232" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C232">
-        <v>9220</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
@@ -3163,7 +3168,7 @@
         <v>62</v>
       </c>
       <c r="B233" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C233">
         <v>0.02</v>
@@ -3171,46 +3176,46 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B234" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C234">
-        <v>0.02</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B235" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C235">
-        <v>0.02</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B236" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C236">
-        <v>0.02</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B237" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C237">
-        <v>0.02</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
@@ -3218,7 +3223,7 @@
         <v>45</v>
       </c>
       <c r="B238" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C238">
         <v>25200</v>
@@ -3226,46 +3231,46 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B239" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C239">
-        <v>25200</v>
+        <v>6.34</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B240" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C240">
-        <v>25200</v>
+        <v>6.34</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B241" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C241">
-        <v>25200</v>
+        <v>6.34</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B242" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C242">
-        <v>25200</v>
+        <v>6.34</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
@@ -3273,7 +3278,7 @@
         <v>58</v>
       </c>
       <c r="B243" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C243">
         <v>6.34</v>
@@ -3281,46 +3286,46 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B244" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C244">
-        <v>6.34</v>
+        <v>4.3999999999999997E-2</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B245" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C245">
-        <v>6.34</v>
+        <v>4.3999999999999997E-2</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B246" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C246">
-        <v>6.34</v>
+        <v>4.3999999999999997E-2</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B247" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C247">
-        <v>6.34</v>
+        <v>4.3999999999999997E-2</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
@@ -3328,7 +3333,7 @@
         <v>59</v>
       </c>
       <c r="B248" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C248">
         <v>4.3999999999999997E-2</v>
@@ -3336,63 +3341,19 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B249" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C249">
-        <v>4.3999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A250" t="s">
-        <v>59</v>
-      </c>
-      <c r="B250" t="s">
-        <v>50</v>
-      </c>
-      <c r="C250">
-        <v>4.3999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A251" t="s">
-        <v>59</v>
-      </c>
-      <c r="B251" t="s">
-        <v>46</v>
-      </c>
-      <c r="C251">
-        <v>4.3999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A252" t="s">
-        <v>59</v>
-      </c>
-      <c r="B252" t="s">
-        <v>48</v>
-      </c>
-      <c r="C252">
-        <v>4.3999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A253" t="s">
-        <v>64</v>
-      </c>
-      <c r="B253" t="s">
-        <v>48</v>
-      </c>
-      <c r="C253">
         <v>4.5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C253" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C253">
-      <sortCondition ref="A1:A944"/>
+  <autoFilter ref="A1:C249" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C249">
+      <sortCondition ref="A1:A940"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>